<commit_message>
Change timer in logic manager to system.timer; update docs
</commit_message>
<xml_diff>
--- a/doc/eco/book2.xlsx
+++ b/doc/eco/book2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="15">
   <si>
     <t>Показатель</t>
-  </si>
-  <si>
-    <t>sum</t>
   </si>
   <si>
     <t>Управление периодом работы</t>
@@ -71,12 +68,15 @@
   <si>
     <t>M2M GPS</t>
   </si>
+  <si>
+    <t>avr</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,14 +91,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
@@ -198,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -209,30 +201,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1256,11 +1250,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="295239520"/>
-        <c:axId val="298493904"/>
+        <c:axId val="206945080"/>
+        <c:axId val="207085160"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="295239520"/>
+        <c:axId val="206945080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,7 +1297,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298493904"/>
+        <c:crossAx val="207085160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1311,7 +1305,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298493904"/>
+        <c:axId val="207085160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,7 +1356,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295239520"/>
+        <c:crossAx val="206945080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1975,11 +1969,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235355640"/>
-        <c:axId val="235356032"/>
+        <c:axId val="206440792"/>
+        <c:axId val="206940608"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="235355640"/>
+        <c:axId val="206440792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2022,7 +2016,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235356032"/>
+        <c:crossAx val="206940608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2030,7 +2024,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235356032"/>
+        <c:axId val="206940608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,7 +2075,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235355640"/>
+        <c:crossAx val="206440792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3369,12 +3363,12 @@
         <c:gapWidth val="160"/>
         <c:gapDepth val="0"/>
         <c:shape val="box"/>
-        <c:axId val="233687336"/>
-        <c:axId val="297059368"/>
-        <c:axId val="453073656"/>
+        <c:axId val="237686416"/>
+        <c:axId val="237644464"/>
+        <c:axId val="238008800"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="233687336"/>
+        <c:axId val="237686416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3411,7 +3405,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297059368"/>
+        <c:crossAx val="237644464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3419,7 +3413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297059368"/>
+        <c:axId val="237644464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3456,12 +3450,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233687336"/>
+        <c:crossAx val="237686416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="453073656"/>
+        <c:axId val="238008800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3497,7 +3491,8 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297059368"/>
+        <c:crossAx val="237644464"/>
+        <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
         <a:noFill/>
@@ -4491,11 +4486,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="441647720"/>
-        <c:axId val="296316632"/>
+        <c:axId val="238169600"/>
+        <c:axId val="206430400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="441647720"/>
+        <c:axId val="238169600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4552,7 +4547,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296316632"/>
+        <c:crossAx val="206430400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4560,7 +4555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296316632"/>
+        <c:axId val="206430400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4571,7 +4566,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="441647720"/>
+        <c:crossAx val="238169600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7279,13 +7274,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47:L53"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="11" width="5.7109375" customWidth="1"/>
     <col min="12" max="12" width="6.85546875" customWidth="1"/>
     <col min="14" max="14" width="19.5703125" customWidth="1"/>
@@ -7326,1921 +7321,1926 @@
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7">
-        <v>1</v>
-      </c>
-      <c r="H2" s="7">
-        <v>1</v>
-      </c>
-      <c r="I2" s="7">
-        <v>1</v>
-      </c>
-      <c r="J2" s="7">
-        <v>1</v>
-      </c>
-      <c r="K2" s="7">
-        <v>1</v>
-      </c>
-      <c r="L2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="10">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+      <c r="K2" s="10">
+        <v>1</v>
+      </c>
+      <c r="L2" s="10">
         <f>AVERAGE(B2:K2)</f>
         <v>1</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9">
-        <v>1</v>
-      </c>
-      <c r="G3" s="9">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9">
-        <v>1</v>
-      </c>
-      <c r="I3" s="9">
-        <v>1</v>
-      </c>
-      <c r="J3" s="9">
-        <v>1</v>
-      </c>
-      <c r="K3" s="9">
-        <v>1</v>
-      </c>
-      <c r="L3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12">
+        <v>1</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1</v>
+      </c>
+      <c r="J3" s="12">
+        <v>1</v>
+      </c>
+      <c r="K3" s="12">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10">
         <f t="shared" ref="L3:L53" si="0">AVERAGE(B3:K3)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9">
-        <v>1</v>
-      </c>
-      <c r="H4" s="9">
-        <v>1</v>
-      </c>
-      <c r="I4" s="9">
-        <v>1</v>
-      </c>
-      <c r="J4" s="9">
-        <v>1</v>
-      </c>
-      <c r="K4" s="9">
-        <v>1</v>
-      </c>
-      <c r="L4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12">
+        <v>1</v>
+      </c>
+      <c r="J4" s="12">
+        <v>1</v>
+      </c>
+      <c r="K4" s="12">
+        <v>1</v>
+      </c>
+      <c r="L4" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9">
-        <v>1</v>
-      </c>
-      <c r="F5" s="9">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9">
-        <v>1</v>
-      </c>
-      <c r="H5" s="9">
-        <v>1</v>
-      </c>
-      <c r="I5" s="9">
-        <v>1</v>
-      </c>
-      <c r="J5" s="9">
-        <v>1</v>
-      </c>
-      <c r="K5" s="9">
-        <v>1</v>
-      </c>
-      <c r="L5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1</v>
+      </c>
+      <c r="I5" s="12">
+        <v>1</v>
+      </c>
+      <c r="J5" s="12">
+        <v>1</v>
+      </c>
+      <c r="K5" s="12">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9">
-        <v>1</v>
-      </c>
-      <c r="E6" s="9">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9">
-        <v>1</v>
-      </c>
-      <c r="G6" s="9">
-        <v>1</v>
-      </c>
-      <c r="H6" s="9">
-        <v>1</v>
-      </c>
-      <c r="I6" s="9">
-        <v>1</v>
-      </c>
-      <c r="J6" s="9">
-        <v>1</v>
-      </c>
-      <c r="K6" s="9">
-        <v>1</v>
-      </c>
-      <c r="L6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1</v>
+      </c>
+      <c r="J6" s="12">
+        <v>1</v>
+      </c>
+      <c r="K6" s="12">
+        <v>1</v>
+      </c>
+      <c r="L6" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0</v>
-      </c>
-      <c r="E7" s="9">
-        <v>0</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-      <c r="G7" s="9">
-        <v>0</v>
-      </c>
-      <c r="H7" s="9">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
-        <v>0</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0</v>
-      </c>
-      <c r="K7" s="9">
-        <v>0</v>
-      </c>
-      <c r="L7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0</v>
+      </c>
+      <c r="L7" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
-      <c r="E8" s="9">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-      <c r="H8" s="9">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9">
-        <v>0</v>
-      </c>
-      <c r="K8" s="9">
-        <v>0</v>
-      </c>
-      <c r="L8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="12"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10">
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
         <v>2</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="6">
         <v>4</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="6">
         <v>5</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="6">
         <v>6</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="6">
         <v>7</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="6">
         <v>8</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="6">
         <v>9</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="6">
         <v>10</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7">
-        <v>1</v>
-      </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7">
-        <v>1</v>
-      </c>
-      <c r="H11" s="7">
-        <v>1</v>
-      </c>
-      <c r="I11" s="7">
-        <v>1</v>
-      </c>
-      <c r="J11" s="7">
-        <v>1</v>
-      </c>
-      <c r="K11" s="7">
-        <v>1</v>
-      </c>
-      <c r="L11" s="7">
+        <v>1</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10">
+        <v>1</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10">
+        <v>1</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1</v>
+      </c>
+      <c r="K11" s="10">
+        <v>1</v>
+      </c>
+      <c r="L11" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="8">
+        <v>2</v>
+      </c>
+      <c r="B12" s="11">
         <v>0.23</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="12">
         <v>0.3</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="12">
         <v>0.21</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="12">
         <v>0.33</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="12">
         <v>0.25</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="12">
         <v>0.19</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="12">
         <v>0.32</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="12">
         <v>0.23</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="12">
         <v>0.22</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="12">
         <v>0.27</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="10">
         <f t="shared" si="0"/>
         <v>0.255</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9">
-        <v>1</v>
-      </c>
-      <c r="E13" s="9">
-        <v>1</v>
-      </c>
-      <c r="F13" s="9">
-        <v>1</v>
-      </c>
-      <c r="G13" s="9">
-        <v>1</v>
-      </c>
-      <c r="H13" s="9">
-        <v>1</v>
-      </c>
-      <c r="I13" s="9">
-        <v>1</v>
-      </c>
-      <c r="J13" s="9">
-        <v>1</v>
-      </c>
-      <c r="K13" s="9">
-        <v>1</v>
-      </c>
-      <c r="L13" s="7">
+        <v>3</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1</v>
+      </c>
+      <c r="E13" s="12">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+      <c r="G13" s="12">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12">
+        <v>1</v>
+      </c>
+      <c r="I13" s="12">
+        <v>1</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1</v>
+      </c>
+      <c r="K13" s="12">
+        <v>1</v>
+      </c>
+      <c r="L13" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="8">
-        <v>1</v>
-      </c>
-      <c r="C14" s="9">
-        <v>1</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1</v>
-      </c>
-      <c r="E14" s="9">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9">
-        <v>1</v>
-      </c>
-      <c r="H14" s="9">
-        <v>1</v>
-      </c>
-      <c r="I14" s="9">
-        <v>1</v>
-      </c>
-      <c r="J14" s="9">
-        <v>1</v>
-      </c>
-      <c r="K14" s="9">
-        <v>1</v>
-      </c>
-      <c r="L14" s="7">
+        <v>4</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12">
+        <v>1</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12">
+        <v>1</v>
+      </c>
+      <c r="K14" s="12">
+        <v>1</v>
+      </c>
+      <c r="L14" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="8">
+        <v>5</v>
+      </c>
+      <c r="B15" s="11">
         <v>0.64</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="12">
         <v>0.72</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="12">
         <v>0.6</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="12">
         <v>0.82</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="12">
         <v>0.59</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="12">
         <v>0.71</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="12">
         <v>0.7</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="12">
         <v>0.63</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="12">
         <v>0.72</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="12">
         <v>0.81</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="10">
         <f t="shared" si="0"/>
         <v>0.69399999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="8">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0</v>
-      </c>
-      <c r="G16" s="9">
-        <v>0</v>
-      </c>
-      <c r="H16" s="9">
-        <v>0</v>
-      </c>
-      <c r="I16" s="9">
-        <v>0</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0</v>
-      </c>
-      <c r="K16" s="9">
-        <v>0</v>
-      </c>
-      <c r="L16" s="7">
+        <v>6</v>
+      </c>
+      <c r="B16" s="11">
+        <v>0</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0</v>
+      </c>
+      <c r="L16" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9">
-        <v>0</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0</v>
-      </c>
-      <c r="E17" s="9">
-        <v>0</v>
-      </c>
-      <c r="F17" s="9">
-        <v>0</v>
-      </c>
-      <c r="G17" s="9">
-        <v>0</v>
-      </c>
-      <c r="H17" s="9">
-        <v>0</v>
-      </c>
-      <c r="I17" s="9">
-        <v>0</v>
-      </c>
-      <c r="J17" s="9">
-        <v>0</v>
-      </c>
-      <c r="K17" s="9">
-        <v>0</v>
-      </c>
-      <c r="L17" s="7">
+        <v>7</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+      <c r="L17" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="12"/>
+      <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="10">
-        <v>1</v>
-      </c>
-      <c r="C19" s="10">
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
         <v>2</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="6">
         <v>3</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="6">
         <v>4</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="6">
         <v>5</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="6">
         <v>6</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="6">
         <v>7</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="6">
         <v>8</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="6">
         <v>9</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="6">
         <v>10</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="6">
-        <v>0</v>
-      </c>
-      <c r="C20" s="7">
-        <v>0</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="7">
-        <v>0</v>
-      </c>
-      <c r="H20" s="7">
-        <v>0</v>
-      </c>
-      <c r="I20" s="7">
-        <v>0</v>
-      </c>
-      <c r="J20" s="7">
-        <v>0</v>
-      </c>
-      <c r="K20" s="7">
-        <v>0</v>
-      </c>
-      <c r="L20" s="7">
+        <v>1</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0</v>
+      </c>
+      <c r="K20" s="10">
+        <v>0</v>
+      </c>
+      <c r="L20" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="8">
+        <v>2</v>
+      </c>
+      <c r="B21" s="11">
         <v>0.31</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="12">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="12">
         <v>0.19</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="12">
         <v>0.32</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="12">
         <v>0.25</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="12">
         <v>0.2</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="12">
         <v>0.31</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="12">
         <v>0.26</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="12">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="12">
         <v>0.31</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="10">
         <f t="shared" si="0"/>
         <v>0.27200000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="8">
-        <v>0</v>
-      </c>
-      <c r="C22" s="9">
-        <v>0</v>
-      </c>
-      <c r="D22" s="9">
-        <v>0</v>
-      </c>
-      <c r="E22" s="9">
-        <v>0</v>
-      </c>
-      <c r="F22" s="9">
-        <v>0</v>
-      </c>
-      <c r="G22" s="9">
-        <v>0</v>
-      </c>
-      <c r="H22" s="9">
-        <v>0</v>
-      </c>
-      <c r="I22" s="9">
-        <v>0</v>
-      </c>
-      <c r="J22" s="9">
-        <v>0</v>
-      </c>
-      <c r="K22" s="9">
-        <v>0</v>
-      </c>
-      <c r="L22" s="7">
+        <v>3</v>
+      </c>
+      <c r="B22" s="11">
+        <v>0</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <v>0</v>
+      </c>
+      <c r="J22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="12">
+        <v>0</v>
+      </c>
+      <c r="L22" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="8">
-        <v>0</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0</v>
-      </c>
-      <c r="E23" s="9">
-        <v>0</v>
-      </c>
-      <c r="F23" s="9">
-        <v>0</v>
-      </c>
-      <c r="G23" s="9">
-        <v>0</v>
-      </c>
-      <c r="H23" s="9">
-        <v>0</v>
-      </c>
-      <c r="I23" s="9">
-        <v>0</v>
-      </c>
-      <c r="J23" s="9">
-        <v>0</v>
-      </c>
-      <c r="K23" s="9">
-        <v>0</v>
-      </c>
-      <c r="L23" s="7">
+        <v>4</v>
+      </c>
+      <c r="B23" s="11">
+        <v>0</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0</v>
+      </c>
+      <c r="G23" s="12">
+        <v>0</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0</v>
+      </c>
+      <c r="I23" s="12">
+        <v>0</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0</v>
+      </c>
+      <c r="K23" s="12">
+        <v>0</v>
+      </c>
+      <c r="L23" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="8">
-        <v>0</v>
-      </c>
-      <c r="C24" s="9">
-        <v>0</v>
-      </c>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-      <c r="E24" s="9">
-        <v>0</v>
-      </c>
-      <c r="F24" s="9">
-        <v>0</v>
-      </c>
-      <c r="G24" s="9">
-        <v>0</v>
-      </c>
-      <c r="H24" s="9">
-        <v>0</v>
-      </c>
-      <c r="I24" s="9">
-        <v>0</v>
-      </c>
-      <c r="J24" s="9">
-        <v>0</v>
-      </c>
-      <c r="K24" s="9">
-        <v>0</v>
-      </c>
-      <c r="L24" s="7">
+        <v>5</v>
+      </c>
+      <c r="B24" s="11">
+        <v>0</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0</v>
+      </c>
+      <c r="I24" s="12">
+        <v>0</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <v>0</v>
+      </c>
+      <c r="L24" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="8">
-        <v>0</v>
-      </c>
-      <c r="C25" s="9">
-        <v>0</v>
-      </c>
-      <c r="D25" s="9">
-        <v>0</v>
-      </c>
-      <c r="E25" s="9">
-        <v>0</v>
-      </c>
-      <c r="F25" s="9">
-        <v>0</v>
-      </c>
-      <c r="G25" s="9">
-        <v>0</v>
-      </c>
-      <c r="H25" s="9">
-        <v>0</v>
-      </c>
-      <c r="I25" s="9">
-        <v>0</v>
-      </c>
-      <c r="J25" s="9">
-        <v>0</v>
-      </c>
-      <c r="K25" s="9">
-        <v>0</v>
-      </c>
-      <c r="L25" s="7">
+        <v>6</v>
+      </c>
+      <c r="B25" s="11">
+        <v>0</v>
+      </c>
+      <c r="C25" s="12">
+        <v>0</v>
+      </c>
+      <c r="D25" s="12">
+        <v>0</v>
+      </c>
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0</v>
+      </c>
+      <c r="I25" s="12">
+        <v>0</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0</v>
+      </c>
+      <c r="K25" s="12">
+        <v>0</v>
+      </c>
+      <c r="L25" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="8">
-        <v>0</v>
-      </c>
-      <c r="C26" s="9">
-        <v>0</v>
-      </c>
-      <c r="D26" s="9">
-        <v>0</v>
-      </c>
-      <c r="E26" s="9">
-        <v>0</v>
-      </c>
-      <c r="F26" s="9">
-        <v>0</v>
-      </c>
-      <c r="G26" s="9">
-        <v>0</v>
-      </c>
-      <c r="H26" s="9">
-        <v>0</v>
-      </c>
-      <c r="I26" s="9">
-        <v>0</v>
-      </c>
-      <c r="J26" s="9">
-        <v>0</v>
-      </c>
-      <c r="K26" s="9">
-        <v>0</v>
-      </c>
-      <c r="L26" s="7">
+        <v>7</v>
+      </c>
+      <c r="B26" s="11">
+        <v>0</v>
+      </c>
+      <c r="C26" s="12">
+        <v>0</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0</v>
+      </c>
+      <c r="I26" s="12">
+        <v>0</v>
+      </c>
+      <c r="J26" s="12">
+        <v>0</v>
+      </c>
+      <c r="K26" s="12">
+        <v>0</v>
+      </c>
+      <c r="L26" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
       <c r="L27" s="13"/>
-      <c r="M27" s="12"/>
+      <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="10">
-        <v>1</v>
-      </c>
-      <c r="C28" s="10">
+      <c r="B28" s="6">
+        <v>1</v>
+      </c>
+      <c r="C28" s="6">
         <v>2</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="6">
         <v>3</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="6">
         <v>4</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="6">
         <v>5</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="6">
         <v>6</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="6">
         <v>7</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="6">
         <v>8</v>
       </c>
-      <c r="J28" s="10">
+      <c r="J28" s="6">
         <v>9</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="6">
         <v>10</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="6">
-        <v>0</v>
-      </c>
-      <c r="C29" s="7">
-        <v>0</v>
-      </c>
-      <c r="D29" s="7">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7">
-        <v>0</v>
-      </c>
-      <c r="F29" s="7">
-        <v>0</v>
-      </c>
-      <c r="G29" s="7">
-        <v>0</v>
-      </c>
-      <c r="H29" s="7">
-        <v>0</v>
-      </c>
-      <c r="I29" s="7">
-        <v>0</v>
-      </c>
-      <c r="J29" s="7">
-        <v>0</v>
-      </c>
-      <c r="K29" s="7">
-        <v>0</v>
-      </c>
-      <c r="L29" s="7">
+        <v>1</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+      <c r="E29" s="10">
+        <v>0</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+      <c r="I29" s="10">
+        <v>0</v>
+      </c>
+      <c r="J29" s="10">
+        <v>0</v>
+      </c>
+      <c r="K29" s="10">
+        <v>0</v>
+      </c>
+      <c r="L29" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="8">
+        <v>2</v>
+      </c>
+      <c r="B30" s="11">
         <v>0.42</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="12">
         <v>0.39</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="12">
         <v>0.5</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="12">
         <v>0.41</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="12">
         <v>0.46</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="12">
         <v>0.51</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="12">
         <v>0.38</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I30" s="12">
         <v>0.43</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="12">
         <v>0.4</v>
       </c>
-      <c r="K30" s="9">
+      <c r="K30" s="12">
         <v>0.5</v>
       </c>
-      <c r="L30" s="7">
+      <c r="L30" s="10">
         <f t="shared" si="0"/>
         <v>0.44000000000000006</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="8">
-        <v>0</v>
-      </c>
-      <c r="C31" s="9">
-        <v>0</v>
-      </c>
-      <c r="D31" s="9">
-        <v>0</v>
-      </c>
-      <c r="E31" s="9">
-        <v>0</v>
-      </c>
-      <c r="F31" s="9">
-        <v>0</v>
-      </c>
-      <c r="G31" s="9">
-        <v>0</v>
-      </c>
-      <c r="H31" s="9">
-        <v>0</v>
-      </c>
-      <c r="I31" s="9">
-        <v>0</v>
-      </c>
-      <c r="J31" s="9">
-        <v>0</v>
-      </c>
-      <c r="K31" s="9">
-        <v>0</v>
-      </c>
-      <c r="L31" s="7">
+        <v>3</v>
+      </c>
+      <c r="B31" s="11">
+        <v>0</v>
+      </c>
+      <c r="C31" s="12">
+        <v>0</v>
+      </c>
+      <c r="D31" s="12">
+        <v>0</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0</v>
+      </c>
+      <c r="F31" s="12">
+        <v>0</v>
+      </c>
+      <c r="G31" s="12">
+        <v>0</v>
+      </c>
+      <c r="H31" s="12">
+        <v>0</v>
+      </c>
+      <c r="I31" s="12">
+        <v>0</v>
+      </c>
+      <c r="J31" s="12">
+        <v>0</v>
+      </c>
+      <c r="K31" s="12">
+        <v>0</v>
+      </c>
+      <c r="L31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="8">
-        <v>0</v>
-      </c>
-      <c r="C32" s="9">
-        <v>0</v>
-      </c>
-      <c r="D32" s="9">
-        <v>0</v>
-      </c>
-      <c r="E32" s="9">
-        <v>0</v>
-      </c>
-      <c r="F32" s="9">
-        <v>0</v>
-      </c>
-      <c r="G32" s="9">
-        <v>0</v>
-      </c>
-      <c r="H32" s="9">
-        <v>0</v>
-      </c>
-      <c r="I32" s="9">
-        <v>0</v>
-      </c>
-      <c r="J32" s="9">
-        <v>0</v>
-      </c>
-      <c r="K32" s="9">
-        <v>0</v>
-      </c>
-      <c r="L32" s="7">
+        <v>4</v>
+      </c>
+      <c r="B32" s="11">
+        <v>0</v>
+      </c>
+      <c r="C32" s="12">
+        <v>0</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0</v>
+      </c>
+      <c r="G32" s="12">
+        <v>0</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0</v>
+      </c>
+      <c r="I32" s="12">
+        <v>0</v>
+      </c>
+      <c r="J32" s="12">
+        <v>0</v>
+      </c>
+      <c r="K32" s="12">
+        <v>0</v>
+      </c>
+      <c r="L32" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="8">
-        <v>0</v>
-      </c>
-      <c r="C33" s="9">
-        <v>0</v>
-      </c>
-      <c r="D33" s="9">
-        <v>0</v>
-      </c>
-      <c r="E33" s="9">
-        <v>0</v>
-      </c>
-      <c r="F33" s="9">
-        <v>0</v>
-      </c>
-      <c r="G33" s="9">
-        <v>0</v>
-      </c>
-      <c r="H33" s="9">
-        <v>0</v>
-      </c>
-      <c r="I33" s="9">
-        <v>0</v>
-      </c>
-      <c r="J33" s="9">
-        <v>0</v>
-      </c>
-      <c r="K33" s="9">
-        <v>0</v>
-      </c>
-      <c r="L33" s="7">
+        <v>5</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0</v>
+      </c>
+      <c r="F33" s="12">
+        <v>0</v>
+      </c>
+      <c r="G33" s="12">
+        <v>0</v>
+      </c>
+      <c r="H33" s="12">
+        <v>0</v>
+      </c>
+      <c r="I33" s="12">
+        <v>0</v>
+      </c>
+      <c r="J33" s="12">
+        <v>0</v>
+      </c>
+      <c r="K33" s="12">
+        <v>0</v>
+      </c>
+      <c r="L33" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="8">
-        <v>0</v>
-      </c>
-      <c r="C34" s="9">
-        <v>0</v>
-      </c>
-      <c r="D34" s="9">
-        <v>0</v>
-      </c>
-      <c r="E34" s="9">
-        <v>0</v>
-      </c>
-      <c r="F34" s="9">
-        <v>0</v>
-      </c>
-      <c r="G34" s="9">
-        <v>0</v>
-      </c>
-      <c r="H34" s="9">
-        <v>0</v>
-      </c>
-      <c r="I34" s="9">
-        <v>0</v>
-      </c>
-      <c r="J34" s="9">
-        <v>0</v>
-      </c>
-      <c r="K34" s="9">
-        <v>0</v>
-      </c>
-      <c r="L34" s="7">
+        <v>6</v>
+      </c>
+      <c r="B34" s="11">
+        <v>0</v>
+      </c>
+      <c r="C34" s="12">
+        <v>0</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0</v>
+      </c>
+      <c r="F34" s="12">
+        <v>0</v>
+      </c>
+      <c r="G34" s="12">
+        <v>0</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0</v>
+      </c>
+      <c r="I34" s="12">
+        <v>0</v>
+      </c>
+      <c r="J34" s="12">
+        <v>0</v>
+      </c>
+      <c r="K34" s="12">
+        <v>0</v>
+      </c>
+      <c r="L34" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="8">
-        <v>1</v>
-      </c>
-      <c r="C35" s="9">
-        <v>1</v>
-      </c>
-      <c r="D35" s="9">
-        <v>1</v>
-      </c>
-      <c r="E35" s="9">
-        <v>1</v>
-      </c>
-      <c r="F35" s="9">
-        <v>1</v>
-      </c>
-      <c r="G35" s="9">
-        <v>1</v>
-      </c>
-      <c r="H35" s="9">
-        <v>1</v>
-      </c>
-      <c r="I35" s="9">
-        <v>1</v>
-      </c>
-      <c r="J35" s="9">
-        <v>1</v>
-      </c>
-      <c r="K35" s="9">
-        <v>1</v>
-      </c>
-      <c r="L35" s="7">
+        <v>7</v>
+      </c>
+      <c r="B35" s="11">
+        <v>1</v>
+      </c>
+      <c r="C35" s="12">
+        <v>1</v>
+      </c>
+      <c r="D35" s="12">
+        <v>1</v>
+      </c>
+      <c r="E35" s="12">
+        <v>1</v>
+      </c>
+      <c r="F35" s="12">
+        <v>1</v>
+      </c>
+      <c r="G35" s="12">
+        <v>1</v>
+      </c>
+      <c r="H35" s="12">
+        <v>1</v>
+      </c>
+      <c r="I35" s="12">
+        <v>1</v>
+      </c>
+      <c r="J35" s="12">
+        <v>1</v>
+      </c>
+      <c r="K35" s="12">
+        <v>1</v>
+      </c>
+      <c r="L35" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
       <c r="L36" s="13"/>
-      <c r="M36" s="12"/>
+      <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="10">
-        <v>1</v>
-      </c>
-      <c r="C37" s="10">
+      <c r="B37" s="6">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6">
         <v>2</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="6">
         <v>3</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="6">
         <v>4</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F37" s="6">
         <v>5</v>
       </c>
-      <c r="G37" s="10">
+      <c r="G37" s="6">
         <v>6</v>
       </c>
-      <c r="H37" s="10">
+      <c r="H37" s="6">
         <v>7</v>
       </c>
-      <c r="I37" s="10">
+      <c r="I37" s="6">
         <v>8</v>
       </c>
-      <c r="J37" s="10">
+      <c r="J37" s="6">
         <v>9</v>
       </c>
-      <c r="K37" s="10">
+      <c r="K37" s="6">
         <v>10</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="6">
-        <v>1</v>
-      </c>
-      <c r="C38" s="7">
-        <v>1</v>
-      </c>
-      <c r="D38" s="7">
-        <v>1</v>
-      </c>
-      <c r="E38" s="7">
-        <v>1</v>
-      </c>
-      <c r="F38" s="7">
-        <v>1</v>
-      </c>
-      <c r="G38" s="7">
-        <v>1</v>
-      </c>
-      <c r="H38" s="7">
-        <v>1</v>
-      </c>
-      <c r="I38" s="7">
-        <v>1</v>
-      </c>
-      <c r="J38" s="7">
-        <v>1</v>
-      </c>
-      <c r="K38" s="7">
-        <v>1</v>
-      </c>
-      <c r="L38" s="7">
+        <v>1</v>
+      </c>
+      <c r="B38" s="9">
+        <v>1</v>
+      </c>
+      <c r="C38" s="10">
+        <v>1</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1</v>
+      </c>
+      <c r="E38" s="10">
+        <v>1</v>
+      </c>
+      <c r="F38" s="10">
+        <v>1</v>
+      </c>
+      <c r="G38" s="10">
+        <v>1</v>
+      </c>
+      <c r="H38" s="10">
+        <v>1</v>
+      </c>
+      <c r="I38" s="10">
+        <v>1</v>
+      </c>
+      <c r="J38" s="10">
+        <v>1</v>
+      </c>
+      <c r="K38" s="10">
+        <v>1</v>
+      </c>
+      <c r="L38" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="8">
+        <v>2</v>
+      </c>
+      <c r="B39" s="11">
         <v>0.84</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="12">
         <v>0.71</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="12">
         <v>0.82</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="12">
         <v>0.75</v>
       </c>
-      <c r="F39" s="9">
+      <c r="F39" s="12">
         <v>0.75</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="12">
         <v>0.71</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="12">
         <v>0.81</v>
       </c>
-      <c r="I39" s="9">
+      <c r="I39" s="12">
         <v>0.69</v>
       </c>
-      <c r="J39" s="9">
+      <c r="J39" s="12">
         <v>0.66</v>
       </c>
-      <c r="K39" s="9">
+      <c r="K39" s="12">
         <v>0.8</v>
       </c>
-      <c r="L39" s="7">
+      <c r="L39" s="10">
         <f t="shared" si="0"/>
         <v>0.754</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="8">
-        <v>1</v>
-      </c>
-      <c r="C40" s="9">
-        <v>1</v>
-      </c>
-      <c r="D40" s="9">
-        <v>1</v>
-      </c>
-      <c r="E40" s="9">
-        <v>1</v>
-      </c>
-      <c r="F40" s="9">
-        <v>1</v>
-      </c>
-      <c r="G40" s="9">
-        <v>1</v>
-      </c>
-      <c r="H40" s="9">
-        <v>1</v>
-      </c>
-      <c r="I40" s="9">
-        <v>1</v>
-      </c>
-      <c r="J40" s="9">
-        <v>1</v>
-      </c>
-      <c r="K40" s="9">
-        <v>1</v>
-      </c>
-      <c r="L40" s="7">
+        <v>3</v>
+      </c>
+      <c r="B40" s="11">
+        <v>1</v>
+      </c>
+      <c r="C40" s="12">
+        <v>1</v>
+      </c>
+      <c r="D40" s="12">
+        <v>1</v>
+      </c>
+      <c r="E40" s="12">
+        <v>1</v>
+      </c>
+      <c r="F40" s="12">
+        <v>1</v>
+      </c>
+      <c r="G40" s="12">
+        <v>1</v>
+      </c>
+      <c r="H40" s="12">
+        <v>1</v>
+      </c>
+      <c r="I40" s="12">
+        <v>1</v>
+      </c>
+      <c r="J40" s="12">
+        <v>1</v>
+      </c>
+      <c r="K40" s="12">
+        <v>1</v>
+      </c>
+      <c r="L40" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="8">
-        <v>0</v>
-      </c>
-      <c r="C41" s="9">
-        <v>0</v>
-      </c>
-      <c r="D41" s="9">
-        <v>0</v>
-      </c>
-      <c r="E41" s="9">
-        <v>0</v>
-      </c>
-      <c r="F41" s="9">
-        <v>0</v>
-      </c>
-      <c r="G41" s="9">
-        <v>0</v>
-      </c>
-      <c r="H41" s="9">
-        <v>0</v>
-      </c>
-      <c r="I41" s="9">
-        <v>0</v>
-      </c>
-      <c r="J41" s="9">
-        <v>0</v>
-      </c>
-      <c r="K41" s="9">
-        <v>0</v>
-      </c>
-      <c r="L41" s="7">
+        <v>4</v>
+      </c>
+      <c r="B41" s="11">
+        <v>0</v>
+      </c>
+      <c r="C41" s="12">
+        <v>0</v>
+      </c>
+      <c r="D41" s="12">
+        <v>0</v>
+      </c>
+      <c r="E41" s="12">
+        <v>0</v>
+      </c>
+      <c r="F41" s="12">
+        <v>0</v>
+      </c>
+      <c r="G41" s="12">
+        <v>0</v>
+      </c>
+      <c r="H41" s="12">
+        <v>0</v>
+      </c>
+      <c r="I41" s="12">
+        <v>0</v>
+      </c>
+      <c r="J41" s="12">
+        <v>0</v>
+      </c>
+      <c r="K41" s="12">
+        <v>0</v>
+      </c>
+      <c r="L41" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" s="8">
+        <v>5</v>
+      </c>
+      <c r="B42" s="11">
         <v>0.54</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="12">
         <v>0.48</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="12">
         <v>0.4</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="12">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F42" s="9">
+      <c r="F42" s="12">
         <v>0.6</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="12">
         <v>0.5</v>
       </c>
-      <c r="H42" s="9">
+      <c r="H42" s="12">
         <v>0.54</v>
       </c>
-      <c r="I42" s="9">
+      <c r="I42" s="12">
         <v>0.59</v>
       </c>
-      <c r="J42" s="9">
+      <c r="J42" s="12">
         <v>0.48</v>
       </c>
-      <c r="K42" s="9">
+      <c r="K42" s="12">
         <v>0.5</v>
       </c>
-      <c r="L42" s="7">
+      <c r="L42" s="10">
         <f t="shared" si="0"/>
         <v>0.51800000000000002</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="8">
-        <v>0</v>
-      </c>
-      <c r="C43" s="9">
-        <v>0</v>
-      </c>
-      <c r="D43" s="9">
-        <v>0</v>
-      </c>
-      <c r="E43" s="9">
-        <v>0</v>
-      </c>
-      <c r="F43" s="9">
-        <v>0</v>
-      </c>
-      <c r="G43" s="9">
-        <v>0</v>
-      </c>
-      <c r="H43" s="9">
-        <v>0</v>
-      </c>
-      <c r="I43" s="9">
-        <v>0</v>
-      </c>
-      <c r="J43" s="9">
-        <v>0</v>
-      </c>
-      <c r="K43" s="9">
-        <v>0</v>
-      </c>
-      <c r="L43" s="7">
+        <v>6</v>
+      </c>
+      <c r="B43" s="11">
+        <v>0</v>
+      </c>
+      <c r="C43" s="12">
+        <v>0</v>
+      </c>
+      <c r="D43" s="12">
+        <v>0</v>
+      </c>
+      <c r="E43" s="12">
+        <v>0</v>
+      </c>
+      <c r="F43" s="12">
+        <v>0</v>
+      </c>
+      <c r="G43" s="12">
+        <v>0</v>
+      </c>
+      <c r="H43" s="12">
+        <v>0</v>
+      </c>
+      <c r="I43" s="12">
+        <v>0</v>
+      </c>
+      <c r="J43" s="12">
+        <v>0</v>
+      </c>
+      <c r="K43" s="12">
+        <v>0</v>
+      </c>
+      <c r="L43" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" s="8">
-        <v>1</v>
-      </c>
-      <c r="C44" s="9">
-        <v>1</v>
-      </c>
-      <c r="D44" s="9">
-        <v>1</v>
-      </c>
-      <c r="E44" s="9">
-        <v>1</v>
-      </c>
-      <c r="F44" s="9">
-        <v>1</v>
-      </c>
-      <c r="G44" s="9">
-        <v>1</v>
-      </c>
-      <c r="H44" s="9">
-        <v>1</v>
-      </c>
-      <c r="I44" s="9">
-        <v>1</v>
-      </c>
-      <c r="J44" s="9">
-        <v>1</v>
-      </c>
-      <c r="K44" s="9">
-        <v>1</v>
-      </c>
-      <c r="L44" s="7">
+        <v>7</v>
+      </c>
+      <c r="B44" s="11">
+        <v>1</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1</v>
+      </c>
+      <c r="D44" s="12">
+        <v>1</v>
+      </c>
+      <c r="E44" s="12">
+        <v>1</v>
+      </c>
+      <c r="F44" s="12">
+        <v>1</v>
+      </c>
+      <c r="G44" s="12">
+        <v>1</v>
+      </c>
+      <c r="H44" s="12">
+        <v>1</v>
+      </c>
+      <c r="I44" s="12">
+        <v>1</v>
+      </c>
+      <c r="J44" s="12">
+        <v>1</v>
+      </c>
+      <c r="K44" s="12">
+        <v>1</v>
+      </c>
+      <c r="L44" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
       <c r="L45" s="13"/>
-      <c r="M45" s="12"/>
+      <c r="M45" s="8"/>
     </row>
     <row r="46" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="10">
-        <v>1</v>
-      </c>
-      <c r="C46" s="10">
+      <c r="B46" s="6">
+        <v>1</v>
+      </c>
+      <c r="C46" s="6">
         <v>2</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="6">
         <v>3</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="6">
         <v>4</v>
       </c>
-      <c r="F46" s="10">
+      <c r="F46" s="6">
         <v>5</v>
       </c>
-      <c r="G46" s="10">
+      <c r="G46" s="6">
         <v>6</v>
       </c>
-      <c r="H46" s="10">
+      <c r="H46" s="6">
         <v>7</v>
       </c>
-      <c r="I46" s="10">
+      <c r="I46" s="6">
         <v>8</v>
       </c>
-      <c r="J46" s="10">
+      <c r="J46" s="6">
         <v>9</v>
       </c>
-      <c r="K46" s="10">
+      <c r="K46" s="6">
         <v>10</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="6">
-        <v>1</v>
-      </c>
-      <c r="C47" s="7">
-        <v>1</v>
-      </c>
-      <c r="D47" s="7">
-        <v>1</v>
-      </c>
-      <c r="E47" s="7">
-        <v>1</v>
-      </c>
-      <c r="F47" s="7">
-        <v>1</v>
-      </c>
-      <c r="G47" s="7">
-        <v>1</v>
-      </c>
-      <c r="H47" s="7">
-        <v>1</v>
-      </c>
-      <c r="I47" s="7">
-        <v>1</v>
-      </c>
-      <c r="J47" s="7">
-        <v>1</v>
-      </c>
-      <c r="K47" s="7">
-        <v>1</v>
-      </c>
-      <c r="L47" s="7">
+        <v>1</v>
+      </c>
+      <c r="B47" s="9">
+        <v>1</v>
+      </c>
+      <c r="C47" s="10">
+        <v>1</v>
+      </c>
+      <c r="D47" s="10">
+        <v>1</v>
+      </c>
+      <c r="E47" s="10">
+        <v>1</v>
+      </c>
+      <c r="F47" s="10">
+        <v>1</v>
+      </c>
+      <c r="G47" s="10">
+        <v>1</v>
+      </c>
+      <c r="H47" s="10">
+        <v>1</v>
+      </c>
+      <c r="I47" s="10">
+        <v>1</v>
+      </c>
+      <c r="J47" s="10">
+        <v>1</v>
+      </c>
+      <c r="K47" s="10">
+        <v>1</v>
+      </c>
+      <c r="L47" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="8">
+        <v>2</v>
+      </c>
+      <c r="B48" s="11">
         <v>0.32</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="12">
         <v>0.33</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="12">
         <v>0.25</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E48" s="12">
         <v>0.21</v>
       </c>
-      <c r="F48" s="9">
+      <c r="F48" s="12">
         <v>0.2</v>
       </c>
-      <c r="G48" s="9">
+      <c r="G48" s="12">
         <v>0.25</v>
       </c>
-      <c r="H48" s="9">
+      <c r="H48" s="12">
         <v>0.15</v>
       </c>
-      <c r="I48" s="9">
+      <c r="I48" s="12">
         <v>0.12</v>
       </c>
-      <c r="J48" s="9">
+      <c r="J48" s="12">
         <v>0.21</v>
       </c>
-      <c r="K48" s="9">
+      <c r="K48" s="12">
         <v>0.18</v>
       </c>
-      <c r="L48" s="7">
+      <c r="L48" s="10">
         <f t="shared" si="0"/>
         <v>0.22200000000000003</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="8">
-        <v>1</v>
-      </c>
-      <c r="C49" s="9">
-        <v>1</v>
-      </c>
-      <c r="D49" s="9">
-        <v>1</v>
-      </c>
-      <c r="E49" s="9">
-        <v>1</v>
-      </c>
-      <c r="F49" s="9">
-        <v>1</v>
-      </c>
-      <c r="G49" s="9">
-        <v>1</v>
-      </c>
-      <c r="H49" s="9">
-        <v>1</v>
-      </c>
-      <c r="I49" s="9">
-        <v>1</v>
-      </c>
-      <c r="J49" s="9">
-        <v>1</v>
-      </c>
-      <c r="K49" s="9">
-        <v>1</v>
-      </c>
-      <c r="L49" s="7">
+        <v>3</v>
+      </c>
+      <c r="B49" s="11">
+        <v>1</v>
+      </c>
+      <c r="C49" s="12">
+        <v>1</v>
+      </c>
+      <c r="D49" s="12">
+        <v>1</v>
+      </c>
+      <c r="E49" s="12">
+        <v>1</v>
+      </c>
+      <c r="F49" s="12">
+        <v>1</v>
+      </c>
+      <c r="G49" s="12">
+        <v>1</v>
+      </c>
+      <c r="H49" s="12">
+        <v>1</v>
+      </c>
+      <c r="I49" s="12">
+        <v>1</v>
+      </c>
+      <c r="J49" s="12">
+        <v>1</v>
+      </c>
+      <c r="K49" s="12">
+        <v>1</v>
+      </c>
+      <c r="L49" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="8">
-        <v>1</v>
-      </c>
-      <c r="C50" s="9">
-        <v>1</v>
-      </c>
-      <c r="D50" s="9">
-        <v>1</v>
-      </c>
-      <c r="E50" s="9">
-        <v>1</v>
-      </c>
-      <c r="F50" s="9">
-        <v>1</v>
-      </c>
-      <c r="G50" s="9">
-        <v>1</v>
-      </c>
-      <c r="H50" s="9">
-        <v>1</v>
-      </c>
-      <c r="I50" s="9">
-        <v>1</v>
-      </c>
-      <c r="J50" s="9">
-        <v>1</v>
-      </c>
-      <c r="K50" s="9">
-        <v>1</v>
-      </c>
-      <c r="L50" s="7">
+        <v>4</v>
+      </c>
+      <c r="B50" s="11">
+        <v>1</v>
+      </c>
+      <c r="C50" s="12">
+        <v>1</v>
+      </c>
+      <c r="D50" s="12">
+        <v>1</v>
+      </c>
+      <c r="E50" s="12">
+        <v>1</v>
+      </c>
+      <c r="F50" s="12">
+        <v>1</v>
+      </c>
+      <c r="G50" s="12">
+        <v>1</v>
+      </c>
+      <c r="H50" s="12">
+        <v>1</v>
+      </c>
+      <c r="I50" s="12">
+        <v>1</v>
+      </c>
+      <c r="J50" s="12">
+        <v>1</v>
+      </c>
+      <c r="K50" s="12">
+        <v>1</v>
+      </c>
+      <c r="L50" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51" s="8">
+        <v>5</v>
+      </c>
+      <c r="B51" s="11">
         <v>0.31</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="12">
         <v>0.59</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="12">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E51" s="12">
         <v>0.39</v>
       </c>
-      <c r="F51" s="9">
+      <c r="F51" s="12">
         <v>0.45</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="12">
         <v>0.52</v>
       </c>
-      <c r="H51" s="9">
+      <c r="H51" s="12">
         <v>0.54</v>
       </c>
-      <c r="I51" s="9">
+      <c r="I51" s="12">
         <v>0.45</v>
       </c>
-      <c r="J51" s="9">
+      <c r="J51" s="12">
         <v>0.5</v>
       </c>
-      <c r="K51" s="9">
+      <c r="K51" s="12">
         <v>0.44</v>
       </c>
-      <c r="L51" s="7">
+      <c r="L51" s="10">
         <f t="shared" si="0"/>
         <v>0.47400000000000009</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52" s="8">
-        <v>1</v>
-      </c>
-      <c r="C52" s="9">
-        <v>1</v>
-      </c>
-      <c r="D52" s="9">
-        <v>1</v>
-      </c>
-      <c r="E52" s="9">
-        <v>1</v>
-      </c>
-      <c r="F52" s="9">
-        <v>1</v>
-      </c>
-      <c r="G52" s="9">
-        <v>1</v>
-      </c>
-      <c r="H52" s="9">
-        <v>1</v>
-      </c>
-      <c r="I52" s="9">
-        <v>1</v>
-      </c>
-      <c r="J52" s="9">
-        <v>1</v>
-      </c>
-      <c r="K52" s="9">
-        <v>1</v>
-      </c>
-      <c r="L52" s="7">
+        <v>6</v>
+      </c>
+      <c r="B52" s="11">
+        <v>1</v>
+      </c>
+      <c r="C52" s="12">
+        <v>1</v>
+      </c>
+      <c r="D52" s="12">
+        <v>1</v>
+      </c>
+      <c r="E52" s="12">
+        <v>1</v>
+      </c>
+      <c r="F52" s="12">
+        <v>1</v>
+      </c>
+      <c r="G52" s="12">
+        <v>1</v>
+      </c>
+      <c r="H52" s="12">
+        <v>1</v>
+      </c>
+      <c r="I52" s="12">
+        <v>1</v>
+      </c>
+      <c r="J52" s="12">
+        <v>1</v>
+      </c>
+      <c r="K52" s="12">
+        <v>1</v>
+      </c>
+      <c r="L52" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B53" s="8">
-        <v>1</v>
-      </c>
-      <c r="C53" s="9">
-        <v>1</v>
-      </c>
-      <c r="D53" s="9">
-        <v>1</v>
-      </c>
-      <c r="E53" s="9">
-        <v>1</v>
-      </c>
-      <c r="F53" s="9">
-        <v>1</v>
-      </c>
-      <c r="G53" s="9">
-        <v>1</v>
-      </c>
-      <c r="H53" s="9">
-        <v>1</v>
-      </c>
-      <c r="I53" s="9">
-        <v>1</v>
-      </c>
-      <c r="J53" s="9">
-        <v>1</v>
-      </c>
-      <c r="K53" s="9">
-        <v>1</v>
-      </c>
-      <c r="L53" s="7">
+        <v>7</v>
+      </c>
+      <c r="B53" s="11">
+        <v>1</v>
+      </c>
+      <c r="C53" s="12">
+        <v>1</v>
+      </c>
+      <c r="D53" s="12">
+        <v>1</v>
+      </c>
+      <c r="E53" s="12">
+        <v>1</v>
+      </c>
+      <c r="F53" s="12">
+        <v>1</v>
+      </c>
+      <c r="G53" s="12">
+        <v>1</v>
+      </c>
+      <c r="H53" s="12">
+        <v>1</v>
+      </c>
+      <c r="I53" s="12">
+        <v>1</v>
+      </c>
+      <c r="J53" s="12">
+        <v>1</v>
+      </c>
+      <c r="K53" s="12">
+        <v>1</v>
+      </c>
+      <c r="L53" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -9256,7 +9256,7 @@
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
-      <c r="L54" s="11"/>
+      <c r="L54" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9269,7 +9269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -9306,7 +9306,7 @@
     </row>
     <row r="2" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -9329,7 +9329,7 @@
     </row>
     <row r="3" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -9352,7 +9352,7 @@
     </row>
     <row r="4" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -9375,7 +9375,7 @@
     </row>
     <row r="5" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -9398,7 +9398,7 @@
     </row>
     <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -9421,7 +9421,7 @@
     </row>
     <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -9444,7 +9444,7 @@
     </row>
     <row r="8" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0</v>

</xml_diff>